<commit_message>
added create a car using excel
</commit_message>
<xml_diff>
--- a/cars.xlsx
+++ b/cars.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/studio2/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esmab\IdeaProjects\Summer2019OnlineTestNGSeleniumProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EA66775-086A-EE43-BDF1-E13C91EA5ECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BC1FB8-CEBD-47DD-9BEF-03BADD3C8083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10240" yWindow="0" windowWidth="21760" windowHeight="18000" xr2:uid="{374DE628-534F-4D4A-BE20-2DAEED418ED8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{374DE628-534F-4D4A-BE20-2DAEED418ED8}"/>
   </bookViews>
   <sheets>
     <sheet name="cars" sheetId="1" r:id="rId1"/>
@@ -51,26 +51,14 @@
     <t>red</t>
   </si>
   <si>
-    <r>
-      <t>Model Year</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="13"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
+    <t>Model Year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -85,13 +73,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <i/>
       <sz val="13"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -144,7 +125,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -443,16 +424,16 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="209" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,7 +447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>

</xml_diff>